<commit_message>
SPD semaforo - Avance arrays
</commit_message>
<xml_diff>
--- a/_Sist_Proc_Datos/SemaforoCod.xlsx
+++ b/_Sist_Proc_Datos/SemaforoCod.xlsx
@@ -10,13 +10,14 @@
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
     <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
     <sheet name="Hoja3" sheetId="3" r:id="rId3"/>
+    <sheet name="Hoja4" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="77">
   <si>
     <t>/// Cantidad total de luces led:</t>
   </si>
@@ -234,27 +235,38 @@
     <t>semaforo 1, estado 3</t>
   </si>
   <si>
-    <t xml:space="preserve">    int semState;</t>
-  </si>
-  <si>
     <t>&lt;= acá cargo  para el semaforo el nro. de estado:</t>
   </si>
   <si>
     <t>static S_State secuencia[STATESQTY][SEMAFOROSQTY];</t>
+  </si>
+  <si>
+    <t>void cargarSecNumber (int secNumber, int semaforo1StateNumber, int semaforo2StateNumber)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    secuencia[secNumber][0] = semaforo1StateNumber;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    secuencia[secNumber][1] = semaforo2StateNumber;</t>
+  </si>
+  <si>
+    <t>void cargarCicloEstados()</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    int semaforoState[SEMAFOROSQTY];</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    int ledStateArray[STATUSQTY][LEDSQTY];</t>
+  </si>
+  <si>
+    <t>int ledPin[LEDSQTY];</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -309,8 +321,8 @@
   </cellStyleXfs>
   <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -624,8 +636,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A36" sqref="A36"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -673,37 +685,40 @@
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>12</v>
+      </c>
       <c r="G7" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>3</v>
-      </c>
       <c r="G8" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>16</v>
+        <v>4</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="G11" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>5</v>
+      </c>
       <c r="G12" t="s">
         <v>11</v>
       </c>
@@ -713,14 +728,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>3</v>
-      </c>
-    </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="G15" s="1" t="s">
         <v>12</v>
@@ -728,86 +738,104 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="2"/>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="2"/>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="2"/>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="2"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+      <c r="F25" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="4" t="s">
+      <c r="F26" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" s="4" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
+      <c r="F27" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="2"/>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F28" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="2"/>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="2" t="s">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" s="2"/>
+      <c r="F30" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="2" t="s">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" s="2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="2" t="s">
+      <c r="D32" t="s">
         <v>68</v>
-      </c>
-      <c r="D32" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A34" s="2" t="s">
         <v>35</v>
-      </c>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
+        <v>69</v>
+      </c>
+      <c r="D36" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
         <v>38</v>
       </c>
-      <c r="C36" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="H37" t="s">
         <v>64</v>
       </c>
@@ -833,7 +861,7 @@
   <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -970,103 +998,79 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G25"/>
+  <dimension ref="A1:G34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>40</v>
-      </c>
-      <c r="D1">
-        <v>1</v>
-      </c>
-      <c r="F1">
-        <v>1</v>
-      </c>
-      <c r="G1">
-        <v>1</v>
+        <v>73</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>41</v>
-      </c>
-      <c r="D2">
-        <f>D1+IF(RIGHT(A2,7)=RIGHT(A1,7),,1)</f>
-        <v>1</v>
-      </c>
-      <c r="F2">
-        <f>F1+IF(RIGHT(A2,5)=RIGHT(A1,5),,1)</f>
-        <v>1</v>
-      </c>
-      <c r="G2">
-        <f>G1+IF(MID(A2,25,3)=MID(A1,25,3),,1)</f>
-        <v>1</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D3">
-        <f t="shared" ref="D3:D24" si="0">D2+IF(RIGHT(A3,7)=RIGHT(A2,7),,1)</f>
         <v>1</v>
       </c>
       <c r="F3">
-        <f t="shared" ref="F3:F24" si="1">F2+IF(RIGHT(A3,5)=RIGHT(A2,5),,1)</f>
         <v>1</v>
       </c>
       <c r="G3">
-        <f t="shared" ref="G3:G24" si="2">G2+IF(MID(A3,25,3)=MID(A2,25,3),,1)</f>
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D4">
-        <f t="shared" si="0"/>
+        <f>D3+IF(RIGHT(A4,7)=RIGHT(A3,7),,1)</f>
         <v>1</v>
       </c>
       <c r="F4">
-        <f t="shared" si="1"/>
+        <f>F3+IF(RIGHT(A4,5)=RIGHT(A3,5),,1)</f>
         <v>1</v>
       </c>
       <c r="G4">
-        <f t="shared" si="2"/>
+        <f>G3+IF(MID(A4,25,3)=MID(A3,25,3),,1)</f>
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D5">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="D5:D26" si="0">D4+IF(RIGHT(A5,7)=RIGHT(A4,7),,1)</f>
         <v>1</v>
       </c>
       <c r="F5">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="F5:F26" si="1">F4+IF(RIGHT(A5,5)=RIGHT(A4,5),,1)</f>
         <v>1</v>
       </c>
       <c r="G5">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="G5:G26" si="2">G4+IF(MID(A5,25,3)=MID(A4,25,3),,1)</f>
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D6">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F6">
         <f t="shared" si="1"/>
@@ -1074,16 +1078,16 @@
       </c>
       <c r="G6">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D7">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F7">
         <f t="shared" si="1"/>
@@ -1091,90 +1095,88 @@
       </c>
       <c r="G7">
         <f t="shared" si="2"/>
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D8">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F8">
         <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="G8">
+        <f t="shared" si="2"/>
         <v>2</v>
-      </c>
-      <c r="G8">
-        <f t="shared" si="2"/>
-        <v>4</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D9">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F9">
         <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="G9">
+        <f t="shared" si="2"/>
         <v>3</v>
-      </c>
-      <c r="G9">
-        <f t="shared" si="2"/>
-        <v>5</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D10">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="F10">
         <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="G10">
+        <f t="shared" si="2"/>
         <v>4</v>
-      </c>
-      <c r="G10">
-        <f t="shared" si="2"/>
-        <v>6</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D11">
         <f t="shared" si="0"/>
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="F11">
         <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="G11">
+        <f t="shared" si="2"/>
         <v>5</v>
       </c>
-      <c r="G11">
-        <f t="shared" si="2"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>49</v>
+      </c>
+      <c r="D12">
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="B12" s="5"/>
-      <c r="C12" s="5"/>
-      <c r="D12" s="5">
-        <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
       <c r="F12">
         <f t="shared" si="1"/>
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="G12">
         <f t="shared" si="2"/>
@@ -1183,41 +1185,43 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D13">
         <f t="shared" si="0"/>
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="F13">
         <f t="shared" si="1"/>
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="G13">
         <f t="shared" si="2"/>
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>53</v>
-      </c>
-      <c r="D14">
-        <f t="shared" si="0"/>
-        <v>9</v>
+      <c r="A14" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="B14" s="5"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="5">
+        <f t="shared" si="0"/>
+        <v>8</v>
       </c>
       <c r="F14">
         <f t="shared" si="1"/>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G14">
         <f t="shared" si="2"/>
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D15">
         <f t="shared" si="0"/>
@@ -1234,7 +1238,7 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D16">
         <f t="shared" si="0"/>
@@ -1251,7 +1255,7 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D17">
         <f t="shared" si="0"/>
@@ -1268,15 +1272,15 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D18">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F18">
         <f t="shared" si="1"/>
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G18">
         <f t="shared" si="2"/>
@@ -1285,15 +1289,15 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D19">
         <f t="shared" si="0"/>
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F19">
         <f t="shared" si="1"/>
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="G19">
         <f t="shared" si="2"/>
@@ -1302,79 +1306,79 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D20">
         <f t="shared" si="0"/>
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F20">
         <f t="shared" si="1"/>
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="G20">
         <f t="shared" si="2"/>
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D21">
         <f t="shared" si="0"/>
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F21">
         <f t="shared" si="1"/>
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="G21">
         <f t="shared" si="2"/>
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D22">
         <f t="shared" si="0"/>
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F22">
         <f t="shared" si="1"/>
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G22">
         <f t="shared" si="2"/>
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D23">
         <f t="shared" si="0"/>
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="F23">
         <f t="shared" si="1"/>
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G23">
         <f t="shared" si="2"/>
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D24">
         <f t="shared" si="0"/>
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="F24">
         <f t="shared" si="1"/>
@@ -1382,12 +1386,89 @@
       </c>
       <c r="G24">
         <f t="shared" si="2"/>
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
+        <v>62</v>
+      </c>
+      <c r="D25">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="F25">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+      <c r="G25">
+        <f t="shared" si="2"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>63</v>
+      </c>
+      <c r="D26">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="F26">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+      <c r="G26">
+        <f t="shared" si="2"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
         <v>25</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>25</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>76</v>
       </c>
     </row>
   </sheetData>

</xml_diff>